<commit_message>
fixed the "No base rate found" issue
</commit_message>
<xml_diff>
--- a/api/data/ScaleFactors.xlsx
+++ b/api/data/ScaleFactors.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DI14984_tw111d" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -32,8 +32,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -397,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -410,171 +411,834 @@
         <v>ScaleCode</v>
       </c>
       <c r="C1" t="str">
+        <v>DateOn</v>
+      </c>
+      <c r="D1" t="str">
+        <v>DateOff</v>
+      </c>
+      <c r="E1" t="str">
         <v>ScaleFactor</v>
-      </c>
-      <c r="D1" t="str">
-        <v>DateOn</v>
-      </c>
-      <c r="E1" t="str">
-        <v>DateOff</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>BASIC</v>
+        <v>AML</v>
       </c>
       <c r="B2" t="str">
-        <v>S</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
+        <v>D</v>
+      </c>
+      <c r="C2" t="str">
+        <v>2023-01-01</v>
       </c>
       <c r="D2" t="str">
-        <v>2023-01-01</v>
-      </c>
-      <c r="E2" t="str">
-        <v>2099-12-31</v>
+        <v>2099-12-31</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>BASIC</v>
+        <v>AML</v>
       </c>
       <c r="B3" t="str">
-        <v>D</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
+        <v>E</v>
+      </c>
+      <c r="C3" t="str">
+        <v>2023-01-01</v>
       </c>
       <c r="D3" t="str">
-        <v>2023-01-01</v>
-      </c>
-      <c r="E3" t="str">
-        <v>2099-12-31</v>
+        <v>2099-12-31</v>
+      </c>
+      <c r="E3">
+        <v>2.56</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>BASIC</v>
+        <v>AML</v>
       </c>
       <c r="B4" t="str">
         <v>F</v>
       </c>
-      <c r="C4">
-        <v>2.5</v>
+      <c r="C4" t="str">
+        <v>2023-01-01</v>
       </c>
       <c r="D4" t="str">
-        <v>2023-01-01</v>
-      </c>
-      <c r="E4" t="str">
-        <v>2099-12-31</v>
+        <v>2099-12-31</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>STANDARD</v>
+        <v>AML</v>
       </c>
       <c r="B5" t="str">
-        <v>S</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
+        <v>P</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2023-01-01</v>
       </c>
       <c r="D5" t="str">
-        <v>2023-01-01</v>
-      </c>
-      <c r="E5" t="str">
-        <v>2099-12-31</v>
+        <v>2099-12-31</v>
+      </c>
+      <c r="E5">
+        <v>1.6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>STANDARD</v>
+        <v>AML</v>
       </c>
       <c r="B6" t="str">
-        <v>D</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
+        <v>Q</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2023-01-01</v>
       </c>
       <c r="D6" t="str">
-        <v>2023-01-01</v>
-      </c>
-      <c r="E6" t="str">
-        <v>2099-12-31</v>
+        <v>2099-12-31</v>
+      </c>
+      <c r="E6">
+        <v>2.048</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>STANDARD</v>
+        <v>AML</v>
       </c>
       <c r="B7" t="str">
-        <v>F</v>
-      </c>
-      <c r="C7">
-        <v>2.5</v>
+        <v>S</v>
+      </c>
+      <c r="C7" t="str">
+        <v>2023-01-01</v>
       </c>
       <c r="D7" t="str">
-        <v>2023-01-01</v>
-      </c>
-      <c r="E7" t="str">
-        <v>2099-12-31</v>
+        <v>2099-12-31</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>PREMIUM</v>
+        <v>BML</v>
       </c>
       <c r="B8" t="str">
-        <v>S</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
+        <v>D</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2023-01-01</v>
       </c>
       <c r="D8" t="str">
-        <v>2023-01-01</v>
-      </c>
-      <c r="E8" t="str">
-        <v>2099-12-31</v>
+        <v>2099-12-31</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>PREMIUM</v>
+        <v>BML</v>
       </c>
       <c r="B9" t="str">
-        <v>D</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
+        <v>E</v>
+      </c>
+      <c r="C9" t="str">
+        <v>2023-01-01</v>
       </c>
       <c r="D9" t="str">
-        <v>2023-01-01</v>
-      </c>
-      <c r="E9" t="str">
-        <v>2099-12-31</v>
+        <v>2099-12-31</v>
+      </c>
+      <c r="E9">
+        <v>2.56</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>PREMIUM</v>
+        <v>BML</v>
       </c>
       <c r="B10" t="str">
         <v>F</v>
       </c>
-      <c r="C10">
-        <v>2.5</v>
+      <c r="C10" t="str">
+        <v>2023-01-01</v>
       </c>
       <c r="D10" t="str">
-        <v>2023-01-01</v>
-      </c>
-      <c r="E10" t="str">
-        <v>2099-12-31</v>
+        <v>2099-12-31</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>BML</v>
+      </c>
+      <c r="B11" t="str">
+        <v>P</v>
+      </c>
+      <c r="C11" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D11" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E11">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>BML</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Q</v>
+      </c>
+      <c r="C12" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D12" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E12">
+        <v>2.048</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>BML</v>
+      </c>
+      <c r="B13" t="str">
+        <v>S</v>
+      </c>
+      <c r="C13" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D13" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>H0A</v>
+      </c>
+      <c r="B14" t="str">
+        <v>D</v>
+      </c>
+      <c r="C14" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D14" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>H0A</v>
+      </c>
+      <c r="B15" t="str">
+        <v>E</v>
+      </c>
+      <c r="C15" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D15" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E15">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>H0A</v>
+      </c>
+      <c r="B16" t="str">
+        <v>F</v>
+      </c>
+      <c r="C16" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D16" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>H0A</v>
+      </c>
+      <c r="B17" t="str">
+        <v>P</v>
+      </c>
+      <c r="C17" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D17" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E17">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>H0A</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Q</v>
+      </c>
+      <c r="C18" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D18" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E18">
+        <v>2.048</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>H0A</v>
+      </c>
+      <c r="B19" t="str">
+        <v>S</v>
+      </c>
+      <c r="C19" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D19" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>HA0</v>
+      </c>
+      <c r="B20" t="str">
+        <v>D</v>
+      </c>
+      <c r="C20" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D20" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>HA0</v>
+      </c>
+      <c r="B21" t="str">
+        <v>E</v>
+      </c>
+      <c r="C21" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D21" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E21">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>HA0</v>
+      </c>
+      <c r="B22" t="str">
+        <v>F</v>
+      </c>
+      <c r="C22" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D22" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E22">
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>HA0</v>
+      </c>
+      <c r="B23" t="str">
+        <v>P</v>
+      </c>
+      <c r="C23" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D23" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E23">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>HA0</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Q</v>
+      </c>
+      <c r="C24" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D24" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E24">
+        <v>2.048</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>HA0</v>
+      </c>
+      <c r="B25" t="str">
+        <v>S</v>
+      </c>
+      <c r="C25" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D25" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>AML</v>
+      </c>
+      <c r="B26" t="str">
+        <v>D</v>
+      </c>
+      <c r="C26" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D26" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>AML</v>
+      </c>
+      <c r="B27" t="str">
+        <v>E</v>
+      </c>
+      <c r="C27" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D27" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E27">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>AML</v>
+      </c>
+      <c r="B28" t="str">
+        <v>F</v>
+      </c>
+      <c r="C28" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D28" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>AML</v>
+      </c>
+      <c r="B29" t="str">
+        <v>P</v>
+      </c>
+      <c r="C29" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D29" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E29">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>AML</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Q</v>
+      </c>
+      <c r="C30" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D30" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E30">
+        <v>2.048</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>AML</v>
+      </c>
+      <c r="B31" t="str">
+        <v>S</v>
+      </c>
+      <c r="C31" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D31" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>BML</v>
+      </c>
+      <c r="B32" t="str">
+        <v>D</v>
+      </c>
+      <c r="C32" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D32" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>BML</v>
+      </c>
+      <c r="B33" t="str">
+        <v>E</v>
+      </c>
+      <c r="C33" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D33" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E33">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>BML</v>
+      </c>
+      <c r="B34" t="str">
+        <v>F</v>
+      </c>
+      <c r="C34" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D34" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>BML</v>
+      </c>
+      <c r="B35" t="str">
+        <v>P</v>
+      </c>
+      <c r="C35" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D35" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E35">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>BML</v>
+      </c>
+      <c r="B36" t="str">
+        <v>Q</v>
+      </c>
+      <c r="C36" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D36" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E36">
+        <v>2.048</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>BML</v>
+      </c>
+      <c r="B37" t="str">
+        <v>S</v>
+      </c>
+      <c r="C37" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D37" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>H0A</v>
+      </c>
+      <c r="B38" t="str">
+        <v>D</v>
+      </c>
+      <c r="C38" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D38" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>H0A</v>
+      </c>
+      <c r="B39" t="str">
+        <v>E</v>
+      </c>
+      <c r="C39" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D39" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E39">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>H0A</v>
+      </c>
+      <c r="B40" t="str">
+        <v>F</v>
+      </c>
+      <c r="C40" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D40" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>H0A</v>
+      </c>
+      <c r="B41" t="str">
+        <v>P</v>
+      </c>
+      <c r="C41" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D41" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E41">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>H0A</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Q</v>
+      </c>
+      <c r="C42" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D42" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E42">
+        <v>2.048</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>H0A</v>
+      </c>
+      <c r="B43" t="str">
+        <v>S</v>
+      </c>
+      <c r="C43" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D43" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>HA0</v>
+      </c>
+      <c r="B44" t="str">
+        <v>D</v>
+      </c>
+      <c r="C44" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D44" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>HA0</v>
+      </c>
+      <c r="B45" t="str">
+        <v>E</v>
+      </c>
+      <c r="C45" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D45" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E45">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>HA0</v>
+      </c>
+      <c r="B46" t="str">
+        <v>F</v>
+      </c>
+      <c r="C46" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D46" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E46">
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>HA0</v>
+      </c>
+      <c r="B47" t="str">
+        <v>P</v>
+      </c>
+      <c r="C47" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D47" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E47">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>HA0</v>
+      </c>
+      <c r="B48" t="str">
+        <v>Q</v>
+      </c>
+      <c r="C48" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D48" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E48">
+        <v>2.048</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>HA0</v>
+      </c>
+      <c r="B49" t="str">
+        <v>S</v>
+      </c>
+      <c r="C49" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="D49" t="str">
+        <v>2099-12-31</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E49"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>